<commit_message>
fix issue with time labeling
</commit_message>
<xml_diff>
--- a/MatlabFunction/Matlab EP4.xlsx
+++ b/MatlabFunction/Matlab EP4.xlsx
@@ -907,16 +907,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CH1" sqref="CH1:CR1"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CG2" sqref="CG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -950,9 +947,6 @@
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
@@ -986,9 +980,6 @@
       <c r="X1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="Z1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1022,9 +1013,6 @@
       <c r="AJ1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AL1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1058,9 +1046,6 @@
       <c r="AV1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AX1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1094,9 +1079,6 @@
       <c r="BH1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="BJ1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1130,9 +1112,6 @@
       <c r="BT1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BU1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="BV1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1166,9 +1145,6 @@
       <c r="CF1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="CG1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="CH1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1180,9 @@
       </c>
     </row>
     <row r="2" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1238,7 +1216,9 @@
       <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="N2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1272,7 +1252,9 @@
       <c r="X2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="1"/>
+      <c r="Y2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="Z2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1306,7 +1288,9 @@
       <c r="AJ2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AK2" s="1"/>
+      <c r="AK2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AL2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1340,7 +1324,9 @@
       <c r="AV2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AW2" s="1"/>
+      <c r="AW2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AX2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1374,7 +1360,9 @@
       <c r="BH2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="BI2" s="1"/>
+      <c r="BI2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="BJ2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1408,7 +1396,9 @@
       <c r="BT2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="BU2" s="1"/>
+      <c r="BU2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="BV2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1442,7 +1432,9 @@
       <c r="CF2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="CG2" s="1"/>
+      <c r="CG2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="CH2" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>